<commit_message>
change focus set to detection target
</commit_message>
<xml_diff>
--- a/paper/Neurotron/Neurotron.xlsx
+++ b/paper/Neurotron/Neurotron.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hux/Bluenetics/Git/Neural/neural-study/paper/Neurotron/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AADE1BDF-48D1-D544-A008-DB23D107C46C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED652B7E-3A2D-2C4F-BB7E-DBAAC0D1EB86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2980" yWindow="2160" windowWidth="28240" windowHeight="18300" xr2:uid="{96CDFF01-02CC-EC42-905F-8D15766AF32D}"/>
   </bookViews>
@@ -53,13 +53,37 @@
     <t>y</t>
   </si>
   <si>
+    <t>t-1</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>t+1</t>
+  </si>
+  <si>
+    <t>t+2</t>
+  </si>
+  <si>
+    <t>t+3</t>
+  </si>
+  <si>
+    <t>Example 4: predictive unstimulated Neurotron</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Example 2: non-predictive, non-depressed </t>
+      <t xml:space="preserve">Example 1: predictive, stimulated </t>
     </r>
     <r>
       <rPr>
         <i/>
-        <sz val="12"/>
+        <sz val="16"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -70,12 +94,12 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Example 1: predictive </t>
+      <t xml:space="preserve">Example 2: non-predictive, non-depressed </t>
     </r>
     <r>
       <rPr>
         <i/>
-        <sz val="12"/>
+        <sz val="16"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -91,7 +115,7 @@
     <r>
       <rPr>
         <i/>
-        <sz val="12"/>
+        <sz val="16"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -100,36 +124,12 @@
       <t>Neurotron</t>
     </r>
   </si>
-  <si>
-    <t>t-1</t>
-  </si>
-  <si>
-    <t>q</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>Example 4: unstimulated Neurotron</t>
-  </si>
-  <si>
-    <t>t+1</t>
-  </si>
-  <si>
-    <t>t+2</t>
-  </si>
-  <si>
-    <t>t+3</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -175,14 +175,6 @@
     <font>
       <i/>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="12"/>
       <color rgb="FFD883FF"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -193,6 +185,21 @@
       <color rgb="FF0070C0"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -350,7 +357,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -406,18 +413,19 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -444,50 +452,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>124509</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>12096</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>364564</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>7468</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Grafik 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1CED400-3117-FC21-AF70-81E02B9B3AD8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6715228" y="3863599"/>
-          <a:ext cx="4348878" cy="3315634"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>58103</xdr:colOff>
       <xdr:row>11</xdr:row>
@@ -497,7 +461,7 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>214333</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>124509</xdr:rowOff>
+      <xdr:rowOff>61009</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -513,7 +477,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -541,7 +505,7 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>219547</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>190914</xdr:rowOff>
+      <xdr:rowOff>127414</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -557,7 +521,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -566,6 +530,94 @@
         <a:xfrm>
           <a:off x="5005294" y="725082"/>
           <a:ext cx="4270266" cy="1258773"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>16602</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>80665</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>188041</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>102512</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Grafik 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C709FFDB-E8E7-C4A5-EB1D-60E512167F9B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4963792" y="3932168"/>
+          <a:ext cx="4280262" cy="1347047"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>41503</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>167207</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>157712</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>104753</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Grafik 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E55382BE-EAC3-D34E-2C62-D74A61CF5EDD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4988693" y="5678841"/>
+          <a:ext cx="4225032" cy="1262745"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -874,27 +926,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47F9B967-481D-9B48-9F66-0DBD51A40DF4}">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="153" zoomScaleNormal="153" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="8" width="5.83203125" customWidth="1"/>
-    <col min="9" max="9" width="13" customWidth="1"/>
+    <col min="9" max="9" width="19.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+    </row>
+    <row r="3" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
-      <c r="B3" s="12" t="s">
-        <v>6</v>
+      <c r="B3" s="25" t="s">
+        <v>13</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
@@ -904,7 +972,7 @@
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
     </row>
-    <row r="4" spans="1:9" ht="5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12"/>
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
@@ -915,33 +983,33 @@
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="12"/>
       <c r="B5" s="4"/>
       <c r="C5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H5" s="11" t="s">
         <v>4</v>
       </c>
       <c r="I5" s="12"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
       <c r="B6" s="17" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C6" s="23">
         <v>0</v>
@@ -964,7 +1032,7 @@
       </c>
       <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="12"/>
       <c r="B7" s="17" t="s">
         <v>1</v>
@@ -989,10 +1057,10 @@
       </c>
       <c r="I7" s="12"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="12"/>
       <c r="B8" s="17" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C8" s="23">
         <v>1</v>
@@ -1015,10 +1083,10 @@
       </c>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="12"/>
       <c r="B9" s="17" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C9" s="23">
         <v>1</v>
@@ -1041,10 +1109,10 @@
       </c>
       <c r="I9" s="12"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="12"/>
       <c r="B10" s="18" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C10" s="24">
         <f>C7</f>
@@ -1069,7 +1137,7 @@
       </c>
       <c r="I10" s="12"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="12"/>
       <c r="B11" s="13"/>
       <c r="C11" s="14"/>
@@ -1080,10 +1148,10 @@
       <c r="H11" s="14"/>
       <c r="I11" s="12"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
-      <c r="B12" s="12" t="s">
-        <v>5</v>
+      <c r="B12" s="25" t="s">
+        <v>14</v>
       </c>
       <c r="C12" s="12"/>
       <c r="D12" s="12"/>
@@ -1093,7 +1161,7 @@
       <c r="H12" s="12"/>
       <c r="I12" s="12"/>
     </row>
-    <row r="13" spans="1:9" ht="5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" ht="5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="12"/>
       <c r="C13" s="12"/>
@@ -1104,33 +1172,33 @@
       <c r="H13" s="12"/>
       <c r="I13" s="12"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="12"/>
       <c r="B14" s="4"/>
       <c r="C14" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>3</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H14" s="11" t="s">
         <v>4</v>
       </c>
       <c r="I14" s="12"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="12"/>
       <c r="B15" s="17" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C15" s="23">
         <v>0</v>
@@ -1153,7 +1221,7 @@
       </c>
       <c r="I15" s="12"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="12"/>
       <c r="B16" s="17" t="s">
         <v>1</v>
@@ -1182,7 +1250,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="12"/>
       <c r="B17" s="17" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C17" s="23">
         <v>1</v>
@@ -1208,7 +1276,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="12"/>
       <c r="B18" s="17" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C18" s="23">
         <v>1</v>
@@ -1234,7 +1302,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="12"/>
       <c r="B19" s="18" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C19" s="24">
         <f>C16</f>
@@ -1269,10 +1337,10 @@
       <c r="H20" s="14"/>
       <c r="I20" s="12"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
-      <c r="B21" s="12" t="s">
-        <v>7</v>
+      <c r="B21" s="25" t="s">
+        <v>15</v>
       </c>
       <c r="C21" s="12"/>
       <c r="D21" s="12"/>
@@ -1300,16 +1368,16 @@
         <v>2</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>3</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H23" s="11" t="s">
         <v>4</v>
@@ -1319,7 +1387,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="12"/>
       <c r="B24" s="17" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C24" s="23">
         <v>0</v>
@@ -1371,33 +1439,57 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="12"/>
       <c r="B26" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" s="23"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="10"/>
+        <v>9</v>
+      </c>
+      <c r="C26" s="23">
+        <v>1</v>
+      </c>
+      <c r="D26" s="21">
+        <v>0</v>
+      </c>
+      <c r="E26" s="8">
+        <v>0</v>
+      </c>
+      <c r="F26" s="19">
+        <v>1</v>
+      </c>
+      <c r="G26" s="9">
+        <v>0</v>
+      </c>
+      <c r="H26" s="10">
+        <v>0</v>
+      </c>
       <c r="I26" s="12"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="12"/>
       <c r="B27" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" s="23"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="10"/>
+        <v>10</v>
+      </c>
+      <c r="C27" s="23">
+        <v>1</v>
+      </c>
+      <c r="D27" s="21">
+        <v>1</v>
+      </c>
+      <c r="E27" s="8">
+        <v>0</v>
+      </c>
+      <c r="F27" s="19">
+        <v>1</v>
+      </c>
+      <c r="G27" s="9">
+        <v>0</v>
+      </c>
+      <c r="H27" s="10">
+        <v>0</v>
+      </c>
       <c r="I27" s="12"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="12"/>
       <c r="B28" s="18" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C28" s="24">
         <f>C25</f>
@@ -1417,8 +1509,7 @@
         <v>0</v>
       </c>
       <c r="H28" s="5">
-        <f>MIN(E28*C28+D28*(1-G28),1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I28" s="12"/>
     </row>
@@ -1433,9 +1524,9 @@
       <c r="H29" s="14"/>
       <c r="I29" s="12"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A30" s="12"/>
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C30" s="12"/>
@@ -1464,16 +1555,16 @@
         <v>2</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>3</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H32" s="11" t="s">
         <v>4</v>
@@ -1483,7 +1574,7 @@
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="12"/>
       <c r="B33" s="17" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C33" s="23">
         <v>0</v>
@@ -1534,33 +1625,57 @@
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="12"/>
       <c r="B35" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C35" s="23"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="15"/>
-      <c r="H35" s="10"/>
+        <v>9</v>
+      </c>
+      <c r="C35" s="23">
+        <v>0</v>
+      </c>
+      <c r="D35" s="21">
+        <v>0</v>
+      </c>
+      <c r="E35" s="8">
+        <v>1</v>
+      </c>
+      <c r="F35" s="19">
+        <v>0</v>
+      </c>
+      <c r="G35" s="15">
+        <v>0</v>
+      </c>
+      <c r="H35" s="10">
+        <v>0</v>
+      </c>
       <c r="I35" s="12"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="12"/>
       <c r="B36" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C36" s="23"/>
-      <c r="D36" s="21"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="15"/>
-      <c r="H36" s="10"/>
+        <v>10</v>
+      </c>
+      <c r="C36" s="23">
+        <v>0</v>
+      </c>
+      <c r="D36" s="21">
+        <v>0</v>
+      </c>
+      <c r="E36" s="8">
+        <v>1</v>
+      </c>
+      <c r="F36" s="19">
+        <v>0</v>
+      </c>
+      <c r="G36" s="15">
+        <v>0</v>
+      </c>
+      <c r="H36" s="10">
+        <v>0</v>
+      </c>
       <c r="I36" s="12"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="12"/>
       <c r="B37" s="18" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C37" s="24">
         <f>C34</f>

</xml_diff>